<commit_message>
add profile page edit security
</commit_message>
<xml_diff>
--- a/src/cypress/downloads/data-tugas-akhir-mahasiswa.xlsx
+++ b/src/cypress/downloads/data-tugas-akhir-mahasiswa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>NIM</t>
   </si>
@@ -29,34 +29,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>farhan12</t>
-  </si>
-  <si>
-    <t>Farhan Asyam</t>
-  </si>
-  <si>
-    <t>D4 Teknik Informatika</t>
+    <t>bagustejo</t>
+  </si>
+  <si>
+    <t>Bagus Tejo</t>
+  </si>
+  <si>
+    <t>D4 Sistem Informasi Bisnis</t>
   </si>
   <si>
     <t>Diterima</t>
-  </si>
-  <si>
-    <t>susipujiastuti</t>
-  </si>
-  <si>
-    <t>Susi Pujiastuti</t>
-  </si>
-  <si>
-    <t>S2 Rekayasa Teknologi Informasi</t>
-  </si>
-  <si>
-    <t>bagustejo</t>
-  </si>
-  <si>
-    <t>Bagus Tejo</t>
-  </si>
-  <si>
-    <t>D4 Sistem Informasi Bisnis</t>
   </si>
   <si>
     <t>adesusilo</t>
@@ -402,7 +384,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,37 +428,9 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>